<commit_message>
Ya están las implementaciones de 3 y 4 que obtienen % adecuados
</commit_message>
<xml_diff>
--- a/Data set/Registro Evaluaciones 2018-2019 [20190903].xlsx
+++ b/Data set/Registro Evaluaciones 2018-2019 [20190903].xlsx
@@ -5172,12 +5172,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5190,15 +5217,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5241,23 +5259,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="94" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5277,12 +5280,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5305,9 +5308,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="89" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="90" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5599,7 +5599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AD41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
@@ -5631,81 +5631,81 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="221" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="244"/>
-      <c r="P2" s="244"/>
-      <c r="Q2" s="244"/>
-      <c r="R2" s="244"/>
-      <c r="S2" s="244"/>
-      <c r="T2" s="244"/>
-      <c r="U2" s="244"/>
-      <c r="V2" s="244"/>
-      <c r="W2" s="244"/>
-      <c r="X2" s="244"/>
-      <c r="Y2" s="244"/>
-      <c r="Z2" s="244"/>
-      <c r="AA2" s="244"/>
-      <c r="AB2" s="244"/>
-      <c r="AC2" s="244"/>
-      <c r="AD2" s="244"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
+      <c r="P2" s="221"/>
+      <c r="Q2" s="221"/>
+      <c r="R2" s="221"/>
+      <c r="S2" s="221"/>
+      <c r="T2" s="221"/>
+      <c r="U2" s="221"/>
+      <c r="V2" s="221"/>
+      <c r="W2" s="221"/>
+      <c r="X2" s="221"/>
+      <c r="Y2" s="221"/>
+      <c r="Z2" s="221"/>
+      <c r="AA2" s="221"/>
+      <c r="AB2" s="221"/>
+      <c r="AC2" s="221"/>
+      <c r="AD2" s="221"/>
     </row>
     <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="221" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="244"/>
-      <c r="D3" s="244"/>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="244"/>
-      <c r="P3" s="244"/>
-      <c r="Q3" s="244"/>
-      <c r="R3" s="244"/>
-      <c r="S3" s="244"/>
-      <c r="T3" s="244"/>
-      <c r="U3" s="244"/>
-      <c r="V3" s="244"/>
-      <c r="W3" s="244"/>
-      <c r="X3" s="244"/>
-      <c r="Y3" s="244"/>
-      <c r="Z3" s="244"/>
-      <c r="AA3" s="244"/>
-      <c r="AB3" s="244"/>
-      <c r="AC3" s="244"/>
-      <c r="AD3" s="244"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="221"/>
+      <c r="J3" s="221"/>
+      <c r="K3" s="221"/>
+      <c r="L3" s="221"/>
+      <c r="M3" s="221"/>
+      <c r="N3" s="221"/>
+      <c r="O3" s="221"/>
+      <c r="P3" s="221"/>
+      <c r="Q3" s="221"/>
+      <c r="R3" s="221"/>
+      <c r="S3" s="221"/>
+      <c r="T3" s="221"/>
+      <c r="U3" s="221"/>
+      <c r="V3" s="221"/>
+      <c r="W3" s="221"/>
+      <c r="X3" s="221"/>
+      <c r="Y3" s="221"/>
+      <c r="Z3" s="221"/>
+      <c r="AA3" s="221"/>
+      <c r="AB3" s="221"/>
+      <c r="AC3" s="221"/>
+      <c r="AD3" s="221"/>
     </row>
     <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="221" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="224" t="s">
+      <c r="A5" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="225"/>
-      <c r="D5" s="226"/>
+      <c r="C5" s="234"/>
+      <c r="D5" s="235"/>
       <c r="E5" s="227" t="s">
         <v>5</v>
       </c>
@@ -5714,7 +5714,7 @@
       <c r="H5" s="228"/>
       <c r="I5" s="228"/>
       <c r="J5" s="229"/>
-      <c r="K5" s="241" t="s">
+      <c r="K5" s="247" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="227" t="s">
@@ -5737,78 +5737,78 @@
       <c r="AA5" s="228"/>
       <c r="AB5" s="228"/>
       <c r="AC5" s="229"/>
-      <c r="AD5" s="221" t="s">
+      <c r="AD5" s="222" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="222"/>
-      <c r="B6" s="230" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="232" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="237" t="s">
+      <c r="A6" s="223"/>
+      <c r="B6" s="236" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="238" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="246" t="s">
+      <c r="E6" s="225" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="239" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="248" t="s">
+      <c r="F6" s="245" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="230" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="239" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="248" t="s">
+      <c r="H6" s="245" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="230" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="237" t="s">
+      <c r="J6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="242"/>
-      <c r="L6" s="234" t="s">
+      <c r="K6" s="248"/>
+      <c r="L6" s="240" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="235"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="235"/>
-      <c r="P6" s="235"/>
-      <c r="Q6" s="236"/>
-      <c r="R6" s="234" t="s">
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="241"/>
+      <c r="P6" s="241"/>
+      <c r="Q6" s="242"/>
+      <c r="R6" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="235"/>
-      <c r="T6" s="235"/>
-      <c r="U6" s="235"/>
-      <c r="V6" s="235"/>
-      <c r="W6" s="236"/>
-      <c r="X6" s="234" t="s">
+      <c r="S6" s="241"/>
+      <c r="T6" s="241"/>
+      <c r="U6" s="241"/>
+      <c r="V6" s="241"/>
+      <c r="W6" s="242"/>
+      <c r="X6" s="240" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="235"/>
-      <c r="Z6" s="235"/>
-      <c r="AA6" s="235"/>
-      <c r="AB6" s="235"/>
-      <c r="AC6" s="236"/>
-      <c r="AD6" s="222"/>
+      <c r="Y6" s="241"/>
+      <c r="Z6" s="241"/>
+      <c r="AA6" s="241"/>
+      <c r="AB6" s="241"/>
+      <c r="AC6" s="242"/>
+      <c r="AD6" s="223"/>
     </row>
     <row r="7" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="223"/>
-      <c r="B7" s="231"/>
-      <c r="C7" s="233"/>
-      <c r="D7" s="238"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="240"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="240"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="238"/>
-      <c r="K7" s="243"/>
+      <c r="A7" s="232"/>
+      <c r="B7" s="237"/>
+      <c r="C7" s="239"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="249"/>
       <c r="L7" s="47" t="s">
         <v>13</v>
       </c>
@@ -5863,7 +5863,7 @@
       <c r="AC7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD7" s="245"/>
+      <c r="AD7" s="224"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="79" t="s">
@@ -8090,13 +8090,6 @@
     <sortCondition ref="A8"/>
   </sortState>
   <mergeCells count="20">
-    <mergeCell ref="B2:AD2"/>
-    <mergeCell ref="B3:AD3"/>
-    <mergeCell ref="AD5:AD7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="L5:AC5"/>
@@ -8110,8 +8103,15 @@
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K5:K7"/>
+    <mergeCell ref="B2:AD2"/>
+    <mergeCell ref="B3:AD3"/>
+    <mergeCell ref="AD5:AD7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
   </mergeCells>
-  <conditionalFormatting sqref="H9 F9 J9 P9:Q9 T9 V9:W9 Z9 AB9:AD9 Z11:Z40 V11:W40 T11:T40 P11:Q40 J11:J40 H11:H40 F11:F40 AB11:AD40 N9:N40">
+  <conditionalFormatting sqref="F9 H9 J9 P9:Q9 T9 V9:W9 Z9 AB9:AD9 Z11:Z40 V11:W40 T11:T40 P11:Q40 J11:J40 H11:H40 F11:F40 AB11:AD40 N9:N40">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -8203,7 +8203,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:AD38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
@@ -8236,81 +8236,81 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="221" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="244"/>
-      <c r="P2" s="244"/>
-      <c r="Q2" s="244"/>
-      <c r="R2" s="244"/>
-      <c r="S2" s="244"/>
-      <c r="T2" s="244"/>
-      <c r="U2" s="244"/>
-      <c r="V2" s="244"/>
-      <c r="W2" s="244"/>
-      <c r="X2" s="244"/>
-      <c r="Y2" s="244"/>
-      <c r="Z2" s="244"/>
-      <c r="AA2" s="244"/>
-      <c r="AB2" s="244"/>
-      <c r="AC2" s="244"/>
-      <c r="AD2" s="244"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
+      <c r="P2" s="221"/>
+      <c r="Q2" s="221"/>
+      <c r="R2" s="221"/>
+      <c r="S2" s="221"/>
+      <c r="T2" s="221"/>
+      <c r="U2" s="221"/>
+      <c r="V2" s="221"/>
+      <c r="W2" s="221"/>
+      <c r="X2" s="221"/>
+      <c r="Y2" s="221"/>
+      <c r="Z2" s="221"/>
+      <c r="AA2" s="221"/>
+      <c r="AB2" s="221"/>
+      <c r="AC2" s="221"/>
+      <c r="AD2" s="221"/>
     </row>
     <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="221" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="244"/>
-      <c r="D3" s="244"/>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="244"/>
-      <c r="P3" s="244"/>
-      <c r="Q3" s="244"/>
-      <c r="R3" s="244"/>
-      <c r="S3" s="244"/>
-      <c r="T3" s="244"/>
-      <c r="U3" s="244"/>
-      <c r="V3" s="244"/>
-      <c r="W3" s="244"/>
-      <c r="X3" s="244"/>
-      <c r="Y3" s="244"/>
-      <c r="Z3" s="244"/>
-      <c r="AA3" s="244"/>
-      <c r="AB3" s="244"/>
-      <c r="AC3" s="244"/>
-      <c r="AD3" s="244"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="221"/>
+      <c r="J3" s="221"/>
+      <c r="K3" s="221"/>
+      <c r="L3" s="221"/>
+      <c r="M3" s="221"/>
+      <c r="N3" s="221"/>
+      <c r="O3" s="221"/>
+      <c r="P3" s="221"/>
+      <c r="Q3" s="221"/>
+      <c r="R3" s="221"/>
+      <c r="S3" s="221"/>
+      <c r="T3" s="221"/>
+      <c r="U3" s="221"/>
+      <c r="V3" s="221"/>
+      <c r="W3" s="221"/>
+      <c r="X3" s="221"/>
+      <c r="Y3" s="221"/>
+      <c r="Z3" s="221"/>
+      <c r="AA3" s="221"/>
+      <c r="AB3" s="221"/>
+      <c r="AC3" s="221"/>
+      <c r="AD3" s="221"/>
     </row>
     <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="221" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="224" t="s">
+      <c r="A5" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="225"/>
-      <c r="D5" s="226"/>
+      <c r="C5" s="234"/>
+      <c r="D5" s="235"/>
       <c r="E5" s="227" t="s">
         <v>5</v>
       </c>
@@ -8319,7 +8319,7 @@
       <c r="H5" s="228"/>
       <c r="I5" s="228"/>
       <c r="J5" s="229"/>
-      <c r="K5" s="241" t="s">
+      <c r="K5" s="247" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="227" t="s">
@@ -8342,78 +8342,78 @@
       <c r="AA5" s="228"/>
       <c r="AB5" s="228"/>
       <c r="AC5" s="229"/>
-      <c r="AD5" s="221" t="s">
+      <c r="AD5" s="222" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="222"/>
-      <c r="B6" s="230" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="232" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="237" t="s">
+      <c r="A6" s="223"/>
+      <c r="B6" s="236" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="238" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="256" t="s">
+      <c r="E6" s="250" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="250" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="254" t="s">
+      <c r="F6" s="251" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="255" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="252" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="254" t="s">
+      <c r="H6" s="253" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="255" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="237" t="s">
+      <c r="J6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="242"/>
-      <c r="L6" s="234" t="s">
+      <c r="K6" s="248"/>
+      <c r="L6" s="240" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="235"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="235"/>
-      <c r="P6" s="235"/>
-      <c r="Q6" s="236"/>
-      <c r="R6" s="234" t="s">
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="241"/>
+      <c r="P6" s="241"/>
+      <c r="Q6" s="242"/>
+      <c r="R6" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="235"/>
-      <c r="T6" s="235"/>
-      <c r="U6" s="235"/>
-      <c r="V6" s="235"/>
-      <c r="W6" s="236"/>
-      <c r="X6" s="234" t="s">
+      <c r="S6" s="241"/>
+      <c r="T6" s="241"/>
+      <c r="U6" s="241"/>
+      <c r="V6" s="241"/>
+      <c r="W6" s="242"/>
+      <c r="X6" s="240" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="235"/>
-      <c r="Z6" s="235"/>
-      <c r="AA6" s="235"/>
-      <c r="AB6" s="235"/>
-      <c r="AC6" s="236"/>
-      <c r="AD6" s="222"/>
+      <c r="Y6" s="241"/>
+      <c r="Z6" s="241"/>
+      <c r="AA6" s="241"/>
+      <c r="AB6" s="241"/>
+      <c r="AC6" s="242"/>
+      <c r="AD6" s="223"/>
     </row>
     <row r="7" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="223"/>
-      <c r="B7" s="231"/>
-      <c r="C7" s="233"/>
-      <c r="D7" s="238"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="251"/>
-      <c r="G7" s="255"/>
-      <c r="H7" s="253"/>
-      <c r="I7" s="255"/>
-      <c r="J7" s="238"/>
-      <c r="K7" s="243"/>
+      <c r="A7" s="232"/>
+      <c r="B7" s="237"/>
+      <c r="C7" s="239"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="252"/>
+      <c r="G7" s="256"/>
+      <c r="H7" s="254"/>
+      <c r="I7" s="256"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="249"/>
       <c r="L7" s="47" t="s">
         <v>13</v>
       </c>
@@ -8468,7 +8468,7 @@
       <c r="AC7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD7" s="245"/>
+      <c r="AD7" s="224"/>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" s="80" t="s">
@@ -10576,6 +10576,10 @@
     <sortCondition ref="A8"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="E6:E7"/>
@@ -10592,10 +10596,6 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:F18 H8:H18 J8:K8 N8:N18 P8:Q18 T8:T18 V8:W18 Z8:Z18 AB8:AD18 AB21:AD24 Z21:Z24 V21:W24 T21:T24 P21:Q24 N21:N24 J21:J24 H21:H24 F21:F24 F26:F27 H26:H27 J26:J27 N26:N27 P26:Q27 T26:T27 V26:W27 Z26:Z27 AB26:AD27 AB30:AD31 Z30:Z31 V30:W31 T30:T31 P30:Q31 N30:N31 J30:J31 H30:H31 F30:F31 F33:F37 H33:H37 J33:J37 N33:N37 P33:Q37 T33:T37 V33:W37 Z33:Z37 AB33:AD37 J9:J18 K9:K37">
     <cfRule type="colorScale" priority="51">
@@ -10868,7 +10868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AL47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
@@ -10905,81 +10905,81 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:38" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="221" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="244"/>
-      <c r="P2" s="244"/>
-      <c r="Q2" s="244"/>
-      <c r="R2" s="244"/>
-      <c r="S2" s="244"/>
-      <c r="T2" s="244"/>
-      <c r="U2" s="244"/>
-      <c r="V2" s="244"/>
-      <c r="W2" s="244"/>
-      <c r="X2" s="244"/>
-      <c r="Y2" s="244"/>
-      <c r="Z2" s="244"/>
-      <c r="AA2" s="244"/>
-      <c r="AB2" s="244"/>
-      <c r="AC2" s="244"/>
-      <c r="AD2" s="244"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
+      <c r="P2" s="221"/>
+      <c r="Q2" s="221"/>
+      <c r="R2" s="221"/>
+      <c r="S2" s="221"/>
+      <c r="T2" s="221"/>
+      <c r="U2" s="221"/>
+      <c r="V2" s="221"/>
+      <c r="W2" s="221"/>
+      <c r="X2" s="221"/>
+      <c r="Y2" s="221"/>
+      <c r="Z2" s="221"/>
+      <c r="AA2" s="221"/>
+      <c r="AB2" s="221"/>
+      <c r="AC2" s="221"/>
+      <c r="AD2" s="221"/>
     </row>
     <row r="3" spans="1:38" ht="18" x14ac:dyDescent="0.3">
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="221" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="244"/>
-      <c r="D3" s="244"/>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="244"/>
-      <c r="P3" s="244"/>
-      <c r="Q3" s="244"/>
-      <c r="R3" s="244"/>
-      <c r="S3" s="244"/>
-      <c r="T3" s="244"/>
-      <c r="U3" s="244"/>
-      <c r="V3" s="244"/>
-      <c r="W3" s="244"/>
-      <c r="X3" s="244"/>
-      <c r="Y3" s="244"/>
-      <c r="Z3" s="244"/>
-      <c r="AA3" s="244"/>
-      <c r="AB3" s="244"/>
-      <c r="AC3" s="244"/>
-      <c r="AD3" s="244"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="221"/>
+      <c r="J3" s="221"/>
+      <c r="K3" s="221"/>
+      <c r="L3" s="221"/>
+      <c r="M3" s="221"/>
+      <c r="N3" s="221"/>
+      <c r="O3" s="221"/>
+      <c r="P3" s="221"/>
+      <c r="Q3" s="221"/>
+      <c r="R3" s="221"/>
+      <c r="S3" s="221"/>
+      <c r="T3" s="221"/>
+      <c r="U3" s="221"/>
+      <c r="V3" s="221"/>
+      <c r="W3" s="221"/>
+      <c r="X3" s="221"/>
+      <c r="Y3" s="221"/>
+      <c r="Z3" s="221"/>
+      <c r="AA3" s="221"/>
+      <c r="AB3" s="221"/>
+      <c r="AC3" s="221"/>
+      <c r="AD3" s="221"/>
     </row>
     <row r="4" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="221" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="224" t="s">
+      <c r="A5" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="225"/>
-      <c r="D5" s="226"/>
+      <c r="C5" s="234"/>
+      <c r="D5" s="235"/>
       <c r="E5" s="227" t="s">
         <v>5</v>
       </c>
@@ -10988,7 +10988,7 @@
       <c r="H5" s="228"/>
       <c r="I5" s="228"/>
       <c r="J5" s="229"/>
-      <c r="K5" s="241" t="s">
+      <c r="K5" s="247" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="227" t="s">
@@ -11011,65 +11011,65 @@
       <c r="AA5" s="228"/>
       <c r="AB5" s="228"/>
       <c r="AC5" s="229"/>
-      <c r="AD5" s="221" t="s">
+      <c r="AD5" s="222" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="222"/>
-      <c r="B6" s="230" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="232" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="237" t="s">
+      <c r="A6" s="223"/>
+      <c r="B6" s="236" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="238" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="246" t="s">
+      <c r="E6" s="225" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="239" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="248" t="s">
+      <c r="F6" s="245" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="230" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="239" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="248" t="s">
+      <c r="H6" s="245" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="230" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="237" t="s">
+      <c r="J6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="242"/>
-      <c r="L6" s="234" t="s">
+      <c r="K6" s="248"/>
+      <c r="L6" s="240" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="235"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="235"/>
-      <c r="P6" s="235"/>
-      <c r="Q6" s="236"/>
-      <c r="R6" s="234" t="s">
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="241"/>
+      <c r="P6" s="241"/>
+      <c r="Q6" s="242"/>
+      <c r="R6" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="235"/>
-      <c r="T6" s="235"/>
-      <c r="U6" s="235"/>
-      <c r="V6" s="235"/>
-      <c r="W6" s="236"/>
-      <c r="X6" s="234" t="s">
+      <c r="S6" s="241"/>
+      <c r="T6" s="241"/>
+      <c r="U6" s="241"/>
+      <c r="V6" s="241"/>
+      <c r="W6" s="242"/>
+      <c r="X6" s="240" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="235"/>
-      <c r="Z6" s="235"/>
-      <c r="AA6" s="235"/>
-      <c r="AB6" s="235"/>
-      <c r="AC6" s="236"/>
-      <c r="AD6" s="222"/>
+      <c r="Y6" s="241"/>
+      <c r="Z6" s="241"/>
+      <c r="AA6" s="241"/>
+      <c r="AB6" s="241"/>
+      <c r="AC6" s="242"/>
+      <c r="AD6" s="223"/>
       <c r="AF6" s="257" t="s">
         <v>159</v>
       </c>
@@ -11081,17 +11081,17 @@
       <c r="AL6" s="257"/>
     </row>
     <row r="7" spans="1:38" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="223"/>
-      <c r="B7" s="231"/>
-      <c r="C7" s="233"/>
-      <c r="D7" s="238"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="240"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="240"/>
-      <c r="I7" s="249"/>
-      <c r="J7" s="238"/>
-      <c r="K7" s="243"/>
+      <c r="A7" s="232"/>
+      <c r="B7" s="237"/>
+      <c r="C7" s="239"/>
+      <c r="D7" s="244"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="244"/>
+      <c r="K7" s="249"/>
       <c r="L7" s="47" t="s">
         <v>13</v>
       </c>
@@ -11146,7 +11146,7 @@
       <c r="AC7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD7" s="245"/>
+      <c r="AD7" s="224"/>
       <c r="AF7" s="17" t="s">
         <v>160</v>
       </c>
@@ -14109,15 +14109,6 @@
     <sortCondition ref="A8"/>
   </sortState>
   <mergeCells count="21">
-    <mergeCell ref="AF6:AL6"/>
-    <mergeCell ref="B2:AD2"/>
-    <mergeCell ref="B3:AD3"/>
-    <mergeCell ref="AD5:AD7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="K5:K7"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="L5:AC5"/>
@@ -14130,6 +14121,15 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="AF6:AL6"/>
+    <mergeCell ref="B2:AD2"/>
+    <mergeCell ref="B3:AD3"/>
+    <mergeCell ref="AD5:AD7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="K5:K7"/>
   </mergeCells>
   <conditionalFormatting sqref="F9:F12 H9:H12 J9:K12 N9:N12 P9:Q12 T9:T12 V9:W12 Z9:Z12 AB9:AD12 AB14:AD15 Z14:Z15 V14:W15 T14:T15 P14:Q15 N14:N15 J14:K15 H14:H15 F14:F15 AB18:AD27 Z18:Z27 V18:W27 T18:T27 P18:Q27 N18:N27 J18:K27 H18:H27 F18:F27 F36:F39 H36:H39 J36:K39 N36:N39 P36:Q39 T36:T39 V36:W39 Z36:Z39 AB36:AD39 AB41:AD46 Z41:Z46 V41:W46 T41:T46 P41:Q46 N41:N46 J41:K46 H41:H46 F41:F46 F30:F34 H30:H34 N30:N34 P30:Q34 T30:T34 V30:W34 Z30:Z34 AB30:AD34 J30:K34">
     <cfRule type="colorScale" priority="72">
@@ -14375,9 +14375,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AL65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A43" sqref="A8:A43"/>
+      <selection pane="topRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14408,90 +14408,90 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="221" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="244"/>
-      <c r="F2" s="244"/>
-      <c r="G2" s="244"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="244"/>
-      <c r="J2" s="244"/>
-      <c r="K2" s="244"/>
-      <c r="L2" s="244"/>
-      <c r="M2" s="244"/>
-      <c r="N2" s="244"/>
-      <c r="O2" s="244"/>
-      <c r="P2" s="244"/>
-      <c r="Q2" s="244"/>
-      <c r="R2" s="244"/>
-      <c r="S2" s="244"/>
-      <c r="T2" s="244"/>
-      <c r="U2" s="244"/>
-      <c r="V2" s="244"/>
-      <c r="W2" s="244"/>
-      <c r="X2" s="244"/>
-      <c r="Y2" s="244"/>
-      <c r="Z2" s="244"/>
-      <c r="AA2" s="244"/>
-      <c r="AB2" s="244"/>
-      <c r="AC2" s="244"/>
-      <c r="AD2" s="244"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="221"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="221"/>
+      <c r="J2" s="221"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
+      <c r="M2" s="221"/>
+      <c r="N2" s="221"/>
+      <c r="O2" s="221"/>
+      <c r="P2" s="221"/>
+      <c r="Q2" s="221"/>
+      <c r="R2" s="221"/>
+      <c r="S2" s="221"/>
+      <c r="T2" s="221"/>
+      <c r="U2" s="221"/>
+      <c r="V2" s="221"/>
+      <c r="W2" s="221"/>
+      <c r="X2" s="221"/>
+      <c r="Y2" s="221"/>
+      <c r="Z2" s="221"/>
+      <c r="AA2" s="221"/>
+      <c r="AB2" s="221"/>
+      <c r="AC2" s="221"/>
+      <c r="AD2" s="221"/>
     </row>
     <row r="3" spans="1:30" ht="18" x14ac:dyDescent="0.3">
-      <c r="B3" s="244" t="s">
+      <c r="B3" s="221" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="244"/>
-      <c r="D3" s="244"/>
-      <c r="E3" s="244"/>
-      <c r="F3" s="244"/>
-      <c r="G3" s="244"/>
-      <c r="H3" s="244"/>
-      <c r="I3" s="244"/>
-      <c r="J3" s="244"/>
-      <c r="K3" s="244"/>
-      <c r="L3" s="244"/>
-      <c r="M3" s="244"/>
-      <c r="N3" s="244"/>
-      <c r="O3" s="244"/>
-      <c r="P3" s="244"/>
-      <c r="Q3" s="244"/>
-      <c r="R3" s="244"/>
-      <c r="S3" s="244"/>
-      <c r="T3" s="244"/>
-      <c r="U3" s="244"/>
-      <c r="V3" s="244"/>
-      <c r="W3" s="244"/>
-      <c r="X3" s="244"/>
-      <c r="Y3" s="244"/>
-      <c r="Z3" s="244"/>
-      <c r="AA3" s="244"/>
-      <c r="AB3" s="244"/>
-      <c r="AC3" s="244"/>
-      <c r="AD3" s="244"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="221"/>
+      <c r="J3" s="221"/>
+      <c r="K3" s="221"/>
+      <c r="L3" s="221"/>
+      <c r="M3" s="221"/>
+      <c r="N3" s="221"/>
+      <c r="O3" s="221"/>
+      <c r="P3" s="221"/>
+      <c r="Q3" s="221"/>
+      <c r="R3" s="221"/>
+      <c r="S3" s="221"/>
+      <c r="T3" s="221"/>
+      <c r="U3" s="221"/>
+      <c r="V3" s="221"/>
+      <c r="W3" s="221"/>
+      <c r="X3" s="221"/>
+      <c r="Y3" s="221"/>
+      <c r="Z3" s="221"/>
+      <c r="AA3" s="221"/>
+      <c r="AB3" s="221"/>
+      <c r="AC3" s="221"/>
+      <c r="AD3" s="221"/>
     </row>
     <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="221" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="224" t="s">
+      <c r="A5" s="222" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="233" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="225"/>
-      <c r="D5" s="226"/>
-      <c r="E5" s="262" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="263"/>
-      <c r="G5" s="263"/>
-      <c r="H5" s="263"/>
-      <c r="I5" s="263"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="241" t="s">
+      <c r="C5" s="234"/>
+      <c r="D5" s="235"/>
+      <c r="E5" s="263" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="264"/>
+      <c r="G5" s="264"/>
+      <c r="H5" s="264"/>
+      <c r="I5" s="264"/>
+      <c r="J5" s="265"/>
+      <c r="K5" s="247" t="s">
         <v>6</v>
       </c>
       <c r="L5" s="227" t="s">
@@ -14514,78 +14514,78 @@
       <c r="AA5" s="228"/>
       <c r="AB5" s="228"/>
       <c r="AC5" s="229"/>
-      <c r="AD5" s="221" t="s">
+      <c r="AD5" s="222" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="222"/>
-      <c r="B6" s="230" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="232" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="237" t="s">
+      <c r="A6" s="223"/>
+      <c r="B6" s="236" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="238" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="256" t="s">
+      <c r="E6" s="250" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="239" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="248" t="s">
+      <c r="F6" s="245" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="230" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="239" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="248" t="s">
+      <c r="H6" s="245" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="230" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="237" t="s">
+      <c r="J6" s="243" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="242"/>
-      <c r="L6" s="234" t="s">
+      <c r="K6" s="248"/>
+      <c r="L6" s="240" t="s">
         <v>7</v>
       </c>
-      <c r="M6" s="235"/>
-      <c r="N6" s="235"/>
-      <c r="O6" s="235"/>
-      <c r="P6" s="235"/>
-      <c r="Q6" s="236"/>
-      <c r="R6" s="234" t="s">
+      <c r="M6" s="241"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="241"/>
+      <c r="P6" s="241"/>
+      <c r="Q6" s="242"/>
+      <c r="R6" s="240" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="235"/>
-      <c r="T6" s="235"/>
-      <c r="U6" s="235"/>
-      <c r="V6" s="235"/>
-      <c r="W6" s="236"/>
-      <c r="X6" s="234" t="s">
+      <c r="S6" s="241"/>
+      <c r="T6" s="241"/>
+      <c r="U6" s="241"/>
+      <c r="V6" s="241"/>
+      <c r="W6" s="242"/>
+      <c r="X6" s="240" t="s">
         <v>9</v>
       </c>
-      <c r="Y6" s="235"/>
-      <c r="Z6" s="235"/>
-      <c r="AA6" s="235"/>
-      <c r="AB6" s="235"/>
-      <c r="AC6" s="236"/>
-      <c r="AD6" s="222"/>
+      <c r="Y6" s="241"/>
+      <c r="Z6" s="241"/>
+      <c r="AA6" s="241"/>
+      <c r="AB6" s="241"/>
+      <c r="AC6" s="242"/>
+      <c r="AD6" s="223"/>
     </row>
     <row r="7" spans="1:30" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="222"/>
-      <c r="B7" s="258"/>
-      <c r="C7" s="259"/>
-      <c r="D7" s="260"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="249"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="265"/>
-      <c r="J7" s="260"/>
-      <c r="K7" s="243"/>
+      <c r="A7" s="223"/>
+      <c r="B7" s="259"/>
+      <c r="C7" s="260"/>
+      <c r="D7" s="261"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="262"/>
+      <c r="G7" s="231"/>
+      <c r="H7" s="262"/>
+      <c r="I7" s="266"/>
+      <c r="J7" s="261"/>
+      <c r="K7" s="249"/>
       <c r="L7" s="100" t="s">
         <v>13</v>
       </c>
@@ -14640,7 +14640,7 @@
       <c r="AC7" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="AD7" s="266"/>
+      <c r="AD7" s="258"/>
     </row>
     <row r="8" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="79" t="s">
@@ -17274,6 +17274,9 @@
       <c r="A48" t="s">
         <v>414</v>
       </c>
+      <c r="F48" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:38" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="80" t="s">
@@ -17622,6 +17625,9 @@
       <c r="A53" t="s">
         <v>415</v>
       </c>
+      <c r="F53" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A54" s="80" t="s">
@@ -17915,6 +17921,9 @@
       <c r="A58" t="s">
         <v>416</v>
       </c>
+      <c r="F58" s="14">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A59" s="80" t="s">
@@ -18065,6 +18074,9 @@
     <row r="61" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>417</v>
+      </c>
+      <c r="F61" s="58">
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:38" x14ac:dyDescent="0.3">
@@ -18288,6 +18300,10 @@
     <sortCondition ref="A8"/>
   </sortState>
   <mergeCells count="20">
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="B2:AD2"/>
     <mergeCell ref="B3:AD3"/>
@@ -18304,13 +18320,9 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="E5:J5"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="I6:I7"/>
   </mergeCells>
   <conditionalFormatting sqref="P8:Q16 F8:F16 H8:H16 J8:K8 N8:N16 T8:T16 V8:W16 Z8:Z16 AB8:AD16 AB18:AD21 Z18:Z21 V18:W21 T18:T21 N18:N21 J18:J21 H18:H21 F18:F21 P18:Q21 P25:Q27 F25:F27 H25:H27 J25:J27 N25:N27 T25:T27 V25:W27 Z25:Z27 AB25:AD27 AB29:AD32 Z29:Z32 V29:W32 T29:T32 N29:N32 J29:J32 H29:H32 F29:F32 P29:Q32 P35:Q43 F35:F43 H35:H43 J35:J43 N35:N43 T35:T43 V35:W43 Z35:Z43 AB35:AD43 J9:J16 K9:K21 K23:K43 P23:Q23 F23 H23 J23 N23 T23 V23:W23 Z23 AB23:AD23">
-    <cfRule type="colorScale" priority="159">
+    <cfRule type="colorScale" priority="163">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18322,7 +18334,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:D16 B18:D21 B25:D25 B26:C43 D26:D42 B23:D23">
-    <cfRule type="colorScale" priority="158">
+    <cfRule type="colorScale" priority="162">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18334,7 +18346,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17:Q17 F17 H17 J17 N17 T17 V17:W17 Z17 AB17:AD17">
-    <cfRule type="colorScale" priority="84">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18346,7 +18358,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:D17">
-    <cfRule type="colorScale" priority="83">
+    <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18358,7 +18370,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB24:AD24 Z24 V24:W24 T24 N24 J24 H24 F24 P24:Q24">
-    <cfRule type="colorScale" priority="81">
+    <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18370,7 +18382,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:D24">
-    <cfRule type="colorScale" priority="80">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18382,7 +18394,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28:Q28 F28 H28 J28 N28 T28 V28:W28 Z28 AB28:AD28">
-    <cfRule type="colorScale" priority="78">
+    <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18394,7 +18406,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8:L21 L23:L43">
-    <cfRule type="iconSet" priority="589">
+    <cfRule type="iconSet" priority="593">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18403,7 +18415,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB33:AD33 Z33 V33:W33 T33 N33 J33 H33 F33 P33:Q33">
-    <cfRule type="colorScale" priority="75">
+    <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18415,6 +18427,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:Q34 F34 H34 J34 N34 T34 V34:W34 Z34 AB34:AD34">
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI22:AJ22">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22">
+    <cfRule type="iconSet" priority="73">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB22:AD22 Z22 V22:W22 T22 N22 J22:K22 H22 F22 P22:Q22">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18426,7 +18471,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI22:AJ22">
+  <conditionalFormatting sqref="B22:D22">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI46:AJ46">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18438,16 +18495,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L22">
-    <cfRule type="iconSet" priority="69">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
+  <conditionalFormatting sqref="B46:D46">
+    <cfRule type="colorScale" priority="67">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB22:AD22 Z22 V22:W22 T22 N22 J22:K22 H22 F22 P22:Q22">
+  <conditionalFormatting sqref="AB46:AD46 Z46 V46:W46 T46 N46 J46:K46 H46 F46 P46:Q46">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18459,56 +18519,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B22:D22">
-    <cfRule type="colorScale" priority="67">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI46:AJ46">
-    <cfRule type="colorScale" priority="66">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46:D46">
-    <cfRule type="colorScale" priority="63">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB46:AD46 Z46 V46:W46 T46 N46 J46:K46 H46 F46 P46:Q46">
-    <cfRule type="colorScale" priority="64">
-      <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="iconSet" priority="65">
+    <cfRule type="iconSet" priority="69">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18516,8 +18528,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F47 H47 J47 P47:Q47 T47 V47:W47 Z47 AB47:AD47 N47">
-    <cfRule type="colorScale" priority="62">
+  <conditionalFormatting sqref="H47 F47 J47 P47:Q47 T47 V47:W47 Z47 AB47:AD47 N47">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18529,7 +18541,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47:D47">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18541,7 +18553,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47">
-    <cfRule type="colorScale" priority="59">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18553,7 +18565,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="iconSet" priority="60">
+    <cfRule type="iconSet" priority="64">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18562,6 +18574,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI49:AJ49">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49">
+    <cfRule type="iconSet" priority="61">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB49:AD49 Z49 V49:W49 T49 N49 J49:K49 H49 F49 P49:Q49">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:D49">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI50:AJ50">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18573,7 +18630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L49">
+  <conditionalFormatting sqref="L50">
     <cfRule type="iconSet" priority="57">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -18582,7 +18639,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB49:AD49 Z49 V49:W49 T49 N49 J49:K49 H49 F49 P49:Q49">
+  <conditionalFormatting sqref="P50:Q50 F50 H50 J50:K50 N50 T50 V50:W50 Z50 AB50:AD50">
     <cfRule type="colorScale" priority="56">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18594,7 +18651,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49:D49">
+  <conditionalFormatting sqref="B50:D50">
     <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18606,7 +18663,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI50:AJ50">
+  <conditionalFormatting sqref="AI51:AJ51">
     <cfRule type="colorScale" priority="54">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18618,7 +18675,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L50">
+  <conditionalFormatting sqref="L51">
     <cfRule type="iconSet" priority="53">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -18627,7 +18684,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P50:Q50 F50 H50 J50:K50 N50 T50 V50:W50 Z50 AB50:AD50">
+  <conditionalFormatting sqref="AB51:AD51 Z51 V51:W51 T51 N51 J51:K51 H51 F51 P51:Q51">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18639,7 +18696,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B50:D50">
+  <conditionalFormatting sqref="B51:D51">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18651,11 +18708,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI51:AJ51">
-    <cfRule type="colorScale" priority="50">
+  <conditionalFormatting sqref="K52">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
         <cfvo type="num" val="5"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -18663,8 +18720,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L51">
-    <cfRule type="iconSet" priority="49">
+  <conditionalFormatting sqref="L52">
+    <cfRule type="iconSet" priority="50">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18672,7 +18729,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB51:AD51 Z51 V51:W51 T51 N51 J51:K51 H51 F51 P51:Q51">
+  <conditionalFormatting sqref="AB52:AD52 Z52 V52:W52 T52 N52 J52 H52 F52 P52:Q52">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18684,7 +18741,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B51:D51">
+  <conditionalFormatting sqref="B52:C52">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18696,8 +18753,41 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K52">
+  <conditionalFormatting sqref="D52">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI54:AJ54">
     <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L54">
+    <cfRule type="iconSet" priority="44">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB54:AD54 Z54 V54:W54 T54 N54 J54:K54 H54 F54 P54:Q54">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18708,40 +18798,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L52">
-    <cfRule type="iconSet" priority="46">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB52:AD52 Z52 V52:W52 T52 N52 J52 H52 F52 P52:Q52">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B52:C52">
-    <cfRule type="colorScale" priority="43">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52">
+  <conditionalFormatting sqref="B54:D54">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18753,29 +18810,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI54:AJ54">
+  <conditionalFormatting sqref="AB54:AD54 Z54 V54:W54 T54 N54 J54:K54 H54 F54 P54:Q54">
     <cfRule type="colorScale" priority="41">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L54">
-    <cfRule type="iconSet" priority="40">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB54:AD54 Z54 V54:W54 T54 N54 J54:K54 H54 F54 P54:Q54">
-    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18787,7 +18823,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:D54">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18798,7 +18834,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB54:AD54 Z54 V54:W54 T54 N54 J54:K54 H54 F54 P54:Q54">
+  <conditionalFormatting sqref="K55">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L55">
+    <cfRule type="iconSet" priority="39">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P55:Q55 F55 H55 J55 N55 T55 V55:W55 Z55 AB55:AD55">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18810,7 +18867,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B54:D54">
+  <conditionalFormatting sqref="B55:C55">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18822,8 +18879,41 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55">
+  <conditionalFormatting sqref="D55">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI56:AJ56">
     <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L56">
+    <cfRule type="iconSet" priority="33">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P56:Q56 F56 H56 J56:K56 N56 T56 V56:W56 Z56 AB56:AD56">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18834,40 +18924,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L55">
-    <cfRule type="iconSet" priority="35">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P55:Q55 F55 H55 J55 N55 T55 V55:W55 Z55 AB55:AD55">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B55:C55">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D55">
+  <conditionalFormatting sqref="B56:D56">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18879,8 +18936,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI56:AJ56">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="H57 F57 N57 P57:Q57 T57 V57:W57 Z57 AB57:AD57 J57:K57">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57:C57">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18891,8 +18960,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L56">
-    <cfRule type="iconSet" priority="29">
+  <conditionalFormatting sqref="L57">
+    <cfRule type="iconSet" priority="30">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18900,19 +18969,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P56:Q56 F56 H56 J56:K56 N56 T56 V56:W56 Z56 AB56:AD56">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -18924,8 +18981,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F57 H57 N57 P57:Q57 T57 V57:W57 Z57 AB57:AD57 J57:K57">
-    <cfRule type="colorScale" priority="25">
+  <conditionalFormatting sqref="AB59:AD59 Z59 V59:W59 T59 P59:Q59 N59 J59:K59 H59 F59">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -18936,8 +18993,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57:C57">
-    <cfRule type="colorScale" priority="24">
+  <conditionalFormatting sqref="B59:D59 AF59:AL59">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18948,8 +19005,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L57">
-    <cfRule type="iconSet" priority="26">
+  <conditionalFormatting sqref="L59">
+    <cfRule type="iconSet" priority="24">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18957,19 +19014,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB59:AD59 Z59 V59:W59 T59 P59:Q59 N59 J59:K59 H59 F59">
+  <conditionalFormatting sqref="K60">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -18981,8 +19026,29 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59:D59 AF59:AL59">
+  <conditionalFormatting sqref="L60">
+    <cfRule type="iconSet" priority="23">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P60:Q60 F60 H60 J60 N60 T60 V60:W60 Z60 AB60:AD60">
     <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B60:C60">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -18993,20 +19059,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L59">
-    <cfRule type="iconSet" priority="20">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K60">
-    <cfRule type="colorScale" priority="18">
+  <conditionalFormatting sqref="D60">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
         <cfvo type="num" val="5"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -19014,16 +19071,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L60">
-    <cfRule type="iconSet" priority="19">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P60:Q60 F60 H60 J60 N60 T60 V60:W60 Z60 AB60:AD60">
+  <conditionalFormatting sqref="K62">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -19035,11 +19083,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B60:C60">
+  <conditionalFormatting sqref="L62">
+    <cfRule type="iconSet" priority="18">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P62:Q62 F62 H62 J62 N62 T62 V62:W62 Z62 AB62:AD62">
     <cfRule type="colorScale" priority="16">
       <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
         <cfvo type="num" val="5"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -19047,7 +19104,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
+  <conditionalFormatting sqref="B62:C62">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19059,7 +19116,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62">
+  <conditionalFormatting sqref="D62">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V63:W63 Z63 T63 P63:Q63 J63 H63 F63 AB63:AD63 N63">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -19071,65 +19140,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L62">
-    <cfRule type="iconSet" priority="14">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P62:Q62 F62 H62 J62 N62 T62 V62:W62 Z62 AB62:AD62">
+  <conditionalFormatting sqref="B63:D63">
     <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B62:C62">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V63:W63 Z63 T63 P63:Q63 J63 H63 F63 AB63:AD63 N63">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="2"/>
-        <cfvo type="num" val="3"/>
-        <cfvo type="num" val="5"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B63:D63">
-    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3.5"/>
@@ -19141,7 +19153,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="2"/>
         <cfvo type="num" val="3"/>
@@ -19153,7 +19165,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63">
-    <cfRule type="iconSet" priority="7">
+    <cfRule type="iconSet" priority="11">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="1"/>
@@ -19162,6 +19174,63 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K64">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L64">
+    <cfRule type="iconSet" priority="9">
+      <iconSet iconSet="3Symbols" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB64:AD64 Z64 V64:W64 T64 N64 J64 H64 F64 P64:Q64">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B64:C64">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="5"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F61">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -19173,16 +19242,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L64">
-    <cfRule type="iconSet" priority="5">
-      <iconSet iconSet="3Symbols" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="1"/>
-        <cfvo type="num" val="2"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB64:AD64 Z64 V64:W64 T64 N64 J64 H64 F64 P64:Q64">
+  <conditionalFormatting sqref="F58">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="2"/>
@@ -19194,11 +19254,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B64:C64">
+  <conditionalFormatting sqref="F53">
     <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
         <cfvo type="num" val="5"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
@@ -19206,11 +19266,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="F48">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3.5"/>
+        <cfvo type="num" val="2"/>
+        <cfvo type="num" val="3"/>
         <cfvo type="num" val="5"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>

</xml_diff>